<commit_message>
Created more stat methods, and a a class
</commit_message>
<xml_diff>
--- a/app_lib/California_Gang_Crime.xlsx
+++ b/app_lib/California_Gang_Crime.xlsx
@@ -5,33 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IAli\Documents\UFO_app\app_lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IAli\Documents\python_crime\app_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2847849-B351-4B7D-9A9A-CB61484F62D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54742768-27C3-4860-A1F2-871138D799DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9708" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="California_Gang_Crime" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">California_Gang_Crime!$B$1:$B$34</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">Robbery </t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Murder</t>
-  </si>
-  <si>
-    <t>Violent crime</t>
   </si>
   <si>
     <t>Year</t>
@@ -876,598 +870,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>1993</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1992</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1991</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1994</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1990</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1995</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>1980</v>
       </c>
-      <c r="B2" s="1">
-        <v>210290</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B8" s="1">
         <v>3411</v>
       </c>
-      <c r="D2" s="1">
-        <v>90420</v>
-      </c>
-      <c r="E2" s="1">
-        <v>23532680</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1989</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>1981</v>
       </c>
-      <c r="B3" s="1">
-        <v>208485</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B10" s="1">
         <v>3143</v>
       </c>
-      <c r="D3" s="1">
-        <v>93781</v>
-      </c>
-      <c r="E3" s="1">
-        <v>24159000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1986</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1988</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1987</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2924</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1996</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>1982</v>
       </c>
-      <c r="B4" s="1">
-        <v>201429</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B15" s="1">
         <v>2779</v>
       </c>
-      <c r="D4" s="1">
-        <v>91988</v>
-      </c>
-      <c r="E4" s="1">
-        <v>24724000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1985</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2770</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1984</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>1983</v>
       </c>
-      <c r="B5" s="1">
-        <v>194491</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B18" s="1">
         <v>2639</v>
       </c>
-      <c r="D5" s="1">
-        <v>85826</v>
-      </c>
-      <c r="E5" s="1">
-        <v>25174000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1984</v>
-      </c>
-      <c r="B6" s="1">
-        <v>195589</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2717</v>
-      </c>
-      <c r="D6" s="1">
-        <v>83924</v>
-      </c>
-      <c r="E6" s="1">
-        <v>25622000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1985</v>
-      </c>
-      <c r="B7" s="1">
-        <v>201763</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2770</v>
-      </c>
-      <c r="D7" s="1">
-        <v>86387</v>
-      </c>
-      <c r="E7" s="1">
-        <v>26365000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1986</v>
-      </c>
-      <c r="B8" s="1">
-        <v>248370</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3038</v>
-      </c>
-      <c r="D8" s="1">
-        <v>92512</v>
-      </c>
-      <c r="E8" s="1">
-        <v>26981000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1987</v>
-      </c>
-      <c r="B9" s="1">
-        <v>253943</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2924</v>
-      </c>
-      <c r="D9" s="1">
-        <v>83341</v>
-      </c>
-      <c r="E9" s="1">
-        <v>27663000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1988</v>
-      </c>
-      <c r="B10" s="1">
-        <v>261912</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2936</v>
-      </c>
-      <c r="D10" s="1">
-        <v>86141</v>
-      </c>
-      <c r="E10" s="1">
-        <v>28168000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1989</v>
-      </c>
-      <c r="B11" s="1">
-        <v>284136</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3158</v>
-      </c>
-      <c r="D11" s="1">
-        <v>96431</v>
-      </c>
-      <c r="E11" s="1">
-        <v>29063000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1990</v>
-      </c>
-      <c r="B12" s="1">
-        <v>311051</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3553</v>
-      </c>
-      <c r="D12" s="1">
-        <v>112208</v>
-      </c>
-      <c r="E12" s="1">
-        <v>29760021</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1991</v>
-      </c>
-      <c r="B13" s="1">
-        <v>331122</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3859</v>
-      </c>
-      <c r="D13" s="1">
-        <v>124939</v>
-      </c>
-      <c r="E13" s="1">
-        <v>30380000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1992</v>
-      </c>
-      <c r="B14" s="1">
-        <v>345624</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3921</v>
-      </c>
-      <c r="D14" s="1">
-        <v>130897</v>
-      </c>
-      <c r="E14" s="1">
-        <v>30867000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1993</v>
-      </c>
-      <c r="B15" s="1">
-        <v>336381</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4096</v>
-      </c>
-      <c r="D15" s="1">
-        <v>126436</v>
-      </c>
-      <c r="E15" s="1">
-        <v>31211000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1994</v>
-      </c>
-      <c r="B16" s="1">
-        <v>318395</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3703</v>
-      </c>
-      <c r="D16" s="1">
-        <v>112160</v>
-      </c>
-      <c r="E16" s="1">
-        <v>31431000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1995</v>
-      </c>
-      <c r="B17" s="1">
-        <v>305154</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3531</v>
-      </c>
-      <c r="D17" s="1">
-        <v>104611</v>
-      </c>
-      <c r="E17" s="1">
-        <v>31589000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1996</v>
-      </c>
-      <c r="B18" s="1">
-        <v>274996</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2916</v>
-      </c>
-      <c r="D18" s="1">
-        <v>94222</v>
-      </c>
-      <c r="E18" s="1">
-        <v>31878000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1997</v>
       </c>
       <c r="B19" s="1">
-        <v>257582</v>
-      </c>
-      <c r="C19" s="1">
         <v>2579</v>
       </c>
-      <c r="D19" s="1">
-        <v>81468</v>
-      </c>
-      <c r="E19" s="1">
-        <v>32268000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
+        <v>2005</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2006</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2003</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2002</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2004</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2007</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2001</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>1998</v>
       </c>
-      <c r="B20" s="1">
-        <v>229883</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B27" s="1">
         <v>2171</v>
       </c>
-      <c r="D20" s="1">
-        <v>68782</v>
-      </c>
-      <c r="E20" s="1">
-        <v>32667000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2008</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2000</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>1999</v>
       </c>
-      <c r="B21" s="1">
-        <v>207879</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B30" s="1">
         <v>2005</v>
       </c>
-      <c r="D21" s="1">
-        <v>60039</v>
-      </c>
-      <c r="E21" s="1">
-        <v>33145121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>2000</v>
-      </c>
-      <c r="B22" s="1">
-        <v>210531</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2079</v>
-      </c>
-      <c r="D22" s="1">
-        <v>60249</v>
-      </c>
-      <c r="E22" s="1">
-        <v>33871648</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>2001</v>
-      </c>
-      <c r="B23" s="1">
-        <v>212867</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2206</v>
-      </c>
-      <c r="D23" s="1">
-        <v>64614</v>
-      </c>
-      <c r="E23" s="1">
-        <v>34600463</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>2002</v>
-      </c>
-      <c r="B24" s="1">
-        <v>208388</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2395</v>
-      </c>
-      <c r="D24" s="1">
-        <v>64968</v>
-      </c>
-      <c r="E24" s="1">
-        <v>35001986</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>2003</v>
-      </c>
-      <c r="B25" s="1">
-        <v>205551</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2407</v>
-      </c>
-      <c r="D25" s="1">
-        <v>63770</v>
-      </c>
-      <c r="E25" s="1">
-        <v>35462712</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>2004</v>
-      </c>
-      <c r="B26" s="1">
-        <v>189175</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2392</v>
-      </c>
-      <c r="D26" s="1">
-        <v>61768</v>
-      </c>
-      <c r="E26" s="1">
-        <v>35842038</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2005</v>
-      </c>
-      <c r="B27" s="1">
-        <v>190178</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2503</v>
-      </c>
-      <c r="D27" s="1">
-        <v>63622</v>
-      </c>
-      <c r="E27" s="1">
-        <v>36154147</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>2006</v>
-      </c>
-      <c r="B28" s="1">
-        <v>194483</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2486</v>
-      </c>
-      <c r="D28" s="1">
-        <v>71142</v>
-      </c>
-      <c r="E28" s="1">
-        <v>36457549</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>2007</v>
-      </c>
-      <c r="B29" s="1">
-        <v>191561</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2262</v>
-      </c>
-      <c r="D29" s="1">
-        <v>70706</v>
-      </c>
-      <c r="E29" s="1">
-        <v>36553215</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>2008</v>
-      </c>
-      <c r="B30" s="1">
-        <v>185329</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2142</v>
-      </c>
-      <c r="D30" s="1">
-        <v>69388</v>
-      </c>
-      <c r="E30" s="1">
-        <v>36756666</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2009</v>
       </c>
       <c r="B31" s="1">
-        <v>174934</v>
-      </c>
-      <c r="C31" s="1">
         <v>1972</v>
       </c>
-      <c r="D31" s="1">
-        <v>64093</v>
-      </c>
-      <c r="E31" s="1">
-        <v>36961664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
+        <v>2012</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>2010</v>
       </c>
-      <c r="B32" s="1">
-        <v>164133</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="B33" s="1">
         <v>1809</v>
       </c>
-      <c r="D32" s="1">
-        <v>58116</v>
-      </c>
-      <c r="E32" s="1">
-        <v>37338198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>2011</v>
       </c>
-      <c r="B33" s="1">
-        <v>154943</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="B34" s="1">
         <v>1792</v>
       </c>
-      <c r="D33" s="1">
-        <v>54291</v>
-      </c>
-      <c r="E33" s="1">
-        <v>37683933</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2012</v>
-      </c>
-      <c r="B34" s="1">
-        <v>160944</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1884</v>
-      </c>
-      <c r="D34" s="1">
-        <v>56521</v>
-      </c>
-      <c r="E34" s="1">
-        <v>38041430</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B34" xr:uid="{73978BF2-DD70-4C6B-AB80-B71337DC582D}">
+    <sortState ref="A2:B34">
+      <sortCondition descending="1" ref="B1:B34"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>